<commit_message>
Recent data with new columns
</commit_message>
<xml_diff>
--- a/data/triageOutput/calibrationOutput.xlsx
+++ b/data/triageOutput/calibrationOutput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelgehrung/Desktop/cytosponge-triage/data/triageOutput/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A27D15-9C20-484D-852D-93E7926180B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6743F88-E0D9-F449-984C-2517CDA7342E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,578 +64,578 @@
     <t>Triage class</t>
   </si>
   <si>
-    <t>BEST2_UCL_0086</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0009</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0039</t>
-  </si>
-  <si>
-    <t>BEST2_NTE_0022</t>
-  </si>
-  <si>
-    <t>BEST2_NTE_0015</t>
-  </si>
-  <si>
-    <t>BEST2_NTE_0017</t>
-  </si>
-  <si>
-    <t>BEST2_NTE_0020</t>
-  </si>
-  <si>
-    <t>BEST2_NTE_0003</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0048</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0052</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0383</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0388</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0480</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0204</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0387</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0390</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0083</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0132</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0017</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0010</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0065</t>
-  </si>
-  <si>
-    <t>BEST2_CDD_0002</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0003</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0008</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0030</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0040</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0019</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0011</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0119</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0127</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0128</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0129</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0151</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0235</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0032</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0049</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0082</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0099</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0112</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0117</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0122</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0184</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0001</t>
-  </si>
-  <si>
-    <t>BEST2_NTE_0007</t>
-  </si>
-  <si>
-    <t>BEST2_POR_0014</t>
-  </si>
-  <si>
-    <t>BEST2_POR_0025</t>
-  </si>
-  <si>
-    <t>BEST2_STY_0004</t>
-  </si>
-  <si>
-    <t>BEST2_STY_0019</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0112</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0068</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0052</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0048</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0059</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0211</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0177</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0171</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0016</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0218</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0233</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0256</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0267</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0257</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0268</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0177</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0069</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0133</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0158</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0186</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0202</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0416</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0437</t>
-  </si>
-  <si>
-    <t>BEST2_CDD_0006</t>
-  </si>
-  <si>
-    <t>BEST2_CDD_0018</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0004</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0019</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0024</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0051</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0055</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0062</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0186</t>
-  </si>
-  <si>
-    <t>BEST2_NTE_0019</t>
-  </si>
-  <si>
-    <t>BEST2_PHH_0005</t>
-  </si>
-  <si>
-    <t>BEST2_STM_0014</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0002</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0027</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0057</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0058</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0066</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0069</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0071</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0083</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0154</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0170</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0176</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0178</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0248</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0249</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0252</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0253</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0261</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0195</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0175</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0193</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0261</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0020</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0150</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0176</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0194</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0141</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0174</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0178</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0196</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0200</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0274</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0295</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0165</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0168</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0170</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0174</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0176</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0194</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0202</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0203</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0204</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0001</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0425</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0427</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0487</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0377</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0391</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0401</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0405</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0408</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0006</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0007</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0357</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0361</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0362</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0365</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0368</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0372</t>
-  </si>
-  <si>
-    <t>BEST2_PBH_0001</t>
-  </si>
-  <si>
-    <t>BEST2_PHH_0002</t>
-  </si>
-  <si>
-    <t>BEST2_PHH_0007</t>
-  </si>
-  <si>
-    <t>BEST2_PHH_0008</t>
-  </si>
-  <si>
-    <t>BEST2_PHH_0010</t>
-  </si>
-  <si>
-    <t>BEST2_POR_0008</t>
-  </si>
-  <si>
-    <t>BEST2_POR_0021</t>
-  </si>
-  <si>
-    <t>BEST2_POR_0023</t>
-  </si>
-  <si>
-    <t>BEST2_POR_0041</t>
-  </si>
-  <si>
-    <t>BEST2_STY_0008</t>
-  </si>
-  <si>
-    <t>BEST2_STY_0011</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0214</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0102</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0105</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0112</t>
-  </si>
-  <si>
-    <t>BEST2_CAM_0321</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0091</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0097</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0099</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0101</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0106</t>
-  </si>
-  <si>
-    <t>BEST2_NEW_0117</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0061</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0062</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0065</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0067</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0086</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0090</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0116</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0145</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0203</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0207</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0209</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0273</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0274</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0275</t>
-  </si>
-  <si>
-    <t>BEST2_WEL_0001</t>
-  </si>
-  <si>
-    <t>BEST2_WEL_0002</t>
-  </si>
-  <si>
-    <t>BEST2_WEL_0005</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0079</t>
-  </si>
-  <si>
-    <t>BEST2_NOT_0080</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0132</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0188</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0271</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0281</t>
-  </si>
-  <si>
-    <t>BEST2_UCL_0285</t>
-  </si>
-  <si>
     <t>Gastric count</t>
   </si>
   <si>
     <t>TFF3 positive count</t>
+  </si>
+  <si>
+    <t>BEST2_C_1</t>
+  </si>
+  <si>
+    <t>BEST2_C_2</t>
+  </si>
+  <si>
+    <t>BEST2_C_3</t>
+  </si>
+  <si>
+    <t>BEST2_C_4</t>
+  </si>
+  <si>
+    <t>BEST2_C_5</t>
+  </si>
+  <si>
+    <t>BEST2_C_6</t>
+  </si>
+  <si>
+    <t>BEST2_C_7</t>
+  </si>
+  <si>
+    <t>BEST2_C_8</t>
+  </si>
+  <si>
+    <t>BEST2_C_9</t>
+  </si>
+  <si>
+    <t>BEST2_C_10</t>
+  </si>
+  <si>
+    <t>BEST2_C_11</t>
+  </si>
+  <si>
+    <t>BEST2_C_12</t>
+  </si>
+  <si>
+    <t>BEST2_C_13</t>
+  </si>
+  <si>
+    <t>BEST2_C_14</t>
+  </si>
+  <si>
+    <t>BEST2_C_15</t>
+  </si>
+  <si>
+    <t>BEST2_C_16</t>
+  </si>
+  <si>
+    <t>BEST2_C_17</t>
+  </si>
+  <si>
+    <t>BEST2_C_18</t>
+  </si>
+  <si>
+    <t>BEST2_C_19</t>
+  </si>
+  <si>
+    <t>BEST2_C_20</t>
+  </si>
+  <si>
+    <t>BEST2_C_21</t>
+  </si>
+  <si>
+    <t>BEST2_C_22</t>
+  </si>
+  <si>
+    <t>BEST2_C_23</t>
+  </si>
+  <si>
+    <t>BEST2_C_24</t>
+  </si>
+  <si>
+    <t>BEST2_C_25</t>
+  </si>
+  <si>
+    <t>BEST2_C_26</t>
+  </si>
+  <si>
+    <t>BEST2_C_27</t>
+  </si>
+  <si>
+    <t>BEST2_C_28</t>
+  </si>
+  <si>
+    <t>BEST2_C_29</t>
+  </si>
+  <si>
+    <t>BEST2_C_30</t>
+  </si>
+  <si>
+    <t>BEST2_C_31</t>
+  </si>
+  <si>
+    <t>BEST2_C_32</t>
+  </si>
+  <si>
+    <t>BEST2_C_33</t>
+  </si>
+  <si>
+    <t>BEST2_C_34</t>
+  </si>
+  <si>
+    <t>BEST2_C_35</t>
+  </si>
+  <si>
+    <t>BEST2_C_36</t>
+  </si>
+  <si>
+    <t>BEST2_C_37</t>
+  </si>
+  <si>
+    <t>BEST2_C_38</t>
+  </si>
+  <si>
+    <t>BEST2_C_39</t>
+  </si>
+  <si>
+    <t>BEST2_C_40</t>
+  </si>
+  <si>
+    <t>BEST2_C_41</t>
+  </si>
+  <si>
+    <t>BEST2_C_42</t>
+  </si>
+  <si>
+    <t>BEST2_C_43</t>
+  </si>
+  <si>
+    <t>BEST2_C_44</t>
+  </si>
+  <si>
+    <t>BEST2_C_45</t>
+  </si>
+  <si>
+    <t>BEST2_C_46</t>
+  </si>
+  <si>
+    <t>BEST2_C_47</t>
+  </si>
+  <si>
+    <t>BEST2_C_48</t>
+  </si>
+  <si>
+    <t>BEST2_C_49</t>
+  </si>
+  <si>
+    <t>BEST2_C_50</t>
+  </si>
+  <si>
+    <t>BEST2_C_51</t>
+  </si>
+  <si>
+    <t>BEST2_C_52</t>
+  </si>
+  <si>
+    <t>BEST2_C_53</t>
+  </si>
+  <si>
+    <t>BEST2_C_54</t>
+  </si>
+  <si>
+    <t>BEST2_C_55</t>
+  </si>
+  <si>
+    <t>BEST2_C_56</t>
+  </si>
+  <si>
+    <t>BEST2_C_57</t>
+  </si>
+  <si>
+    <t>BEST2_C_58</t>
+  </si>
+  <si>
+    <t>BEST2_C_59</t>
+  </si>
+  <si>
+    <t>BEST2_C_60</t>
+  </si>
+  <si>
+    <t>BEST2_C_61</t>
+  </si>
+  <si>
+    <t>BEST2_C_62</t>
+  </si>
+  <si>
+    <t>BEST2_C_63</t>
+  </si>
+  <si>
+    <t>BEST2_C_64</t>
+  </si>
+  <si>
+    <t>BEST2_C_65</t>
+  </si>
+  <si>
+    <t>BEST2_C_66</t>
+  </si>
+  <si>
+    <t>BEST2_C_67</t>
+  </si>
+  <si>
+    <t>BEST2_C_68</t>
+  </si>
+  <si>
+    <t>BEST2_C_69</t>
+  </si>
+  <si>
+    <t>BEST2_C_70</t>
+  </si>
+  <si>
+    <t>BEST2_C_71</t>
+  </si>
+  <si>
+    <t>BEST2_C_72</t>
+  </si>
+  <si>
+    <t>BEST2_C_73</t>
+  </si>
+  <si>
+    <t>BEST2_C_74</t>
+  </si>
+  <si>
+    <t>BEST2_C_75</t>
+  </si>
+  <si>
+    <t>BEST2_C_76</t>
+  </si>
+  <si>
+    <t>BEST2_C_77</t>
+  </si>
+  <si>
+    <t>BEST2_C_78</t>
+  </si>
+  <si>
+    <t>BEST2_C_79</t>
+  </si>
+  <si>
+    <t>BEST2_C_80</t>
+  </si>
+  <si>
+    <t>BEST2_C_81</t>
+  </si>
+  <si>
+    <t>BEST2_C_82</t>
+  </si>
+  <si>
+    <t>BEST2_C_83</t>
+  </si>
+  <si>
+    <t>BEST2_C_84</t>
+  </si>
+  <si>
+    <t>BEST2_C_85</t>
+  </si>
+  <si>
+    <t>BEST2_C_86</t>
+  </si>
+  <si>
+    <t>BEST2_C_87</t>
+  </si>
+  <si>
+    <t>BEST2_C_88</t>
+  </si>
+  <si>
+    <t>BEST2_C_89</t>
+  </si>
+  <si>
+    <t>BEST2_C_90</t>
+  </si>
+  <si>
+    <t>BEST2_C_91</t>
+  </si>
+  <si>
+    <t>BEST2_C_92</t>
+  </si>
+  <si>
+    <t>BEST2_C_93</t>
+  </si>
+  <si>
+    <t>BEST2_C_94</t>
+  </si>
+  <si>
+    <t>BEST2_C_95</t>
+  </si>
+  <si>
+    <t>BEST2_C_96</t>
+  </si>
+  <si>
+    <t>BEST2_C_97</t>
+  </si>
+  <si>
+    <t>BEST2_C_98</t>
+  </si>
+  <si>
+    <t>BEST2_C_99</t>
+  </si>
+  <si>
+    <t>BEST2_C_100</t>
+  </si>
+  <si>
+    <t>BEST2_C_101</t>
+  </si>
+  <si>
+    <t>BEST2_C_102</t>
+  </si>
+  <si>
+    <t>BEST2_C_103</t>
+  </si>
+  <si>
+    <t>BEST2_C_104</t>
+  </si>
+  <si>
+    <t>BEST2_C_105</t>
+  </si>
+  <si>
+    <t>BEST2_C_106</t>
+  </si>
+  <si>
+    <t>BEST2_C_107</t>
+  </si>
+  <si>
+    <t>BEST2_C_108</t>
+  </si>
+  <si>
+    <t>BEST2_C_109</t>
+  </si>
+  <si>
+    <t>BEST2_C_110</t>
+  </si>
+  <si>
+    <t>BEST2_C_111</t>
+  </si>
+  <si>
+    <t>BEST2_C_112</t>
+  </si>
+  <si>
+    <t>BEST2_C_113</t>
+  </si>
+  <si>
+    <t>BEST2_C_114</t>
+  </si>
+  <si>
+    <t>BEST2_C_115</t>
+  </si>
+  <si>
+    <t>BEST2_C_116</t>
+  </si>
+  <si>
+    <t>BEST2_C_117</t>
+  </si>
+  <si>
+    <t>BEST2_C_118</t>
+  </si>
+  <si>
+    <t>BEST2_C_119</t>
+  </si>
+  <si>
+    <t>BEST2_C_120</t>
+  </si>
+  <si>
+    <t>BEST2_C_121</t>
+  </si>
+  <si>
+    <t>BEST2_C_122</t>
+  </si>
+  <si>
+    <t>BEST2_C_123</t>
+  </si>
+  <si>
+    <t>BEST2_C_124</t>
+  </si>
+  <si>
+    <t>BEST2_C_125</t>
+  </si>
+  <si>
+    <t>BEST2_C_126</t>
+  </si>
+  <si>
+    <t>BEST2_C_127</t>
+  </si>
+  <si>
+    <t>BEST2_C_128</t>
+  </si>
+  <si>
+    <t>BEST2_C_129</t>
+  </si>
+  <si>
+    <t>BEST2_C_130</t>
+  </si>
+  <si>
+    <t>BEST2_C_131</t>
+  </si>
+  <si>
+    <t>BEST2_C_132</t>
+  </si>
+  <si>
+    <t>BEST2_C_133</t>
+  </si>
+  <si>
+    <t>BEST2_C_134</t>
+  </si>
+  <si>
+    <t>BEST2_C_135</t>
+  </si>
+  <si>
+    <t>BEST2_C_136</t>
+  </si>
+  <si>
+    <t>BEST2_C_137</t>
+  </si>
+  <si>
+    <t>BEST2_C_138</t>
+  </si>
+  <si>
+    <t>BEST2_C_139</t>
+  </si>
+  <si>
+    <t>BEST2_C_140</t>
+  </si>
+  <si>
+    <t>BEST2_C_141</t>
+  </si>
+  <si>
+    <t>BEST2_C_142</t>
+  </si>
+  <si>
+    <t>BEST2_C_143</t>
+  </si>
+  <si>
+    <t>BEST2_C_144</t>
+  </si>
+  <si>
+    <t>BEST2_C_145</t>
+  </si>
+  <si>
+    <t>BEST2_C_146</t>
+  </si>
+  <si>
+    <t>BEST2_C_147</t>
+  </si>
+  <si>
+    <t>BEST2_C_148</t>
+  </si>
+  <si>
+    <t>BEST2_C_149</t>
+  </si>
+  <si>
+    <t>BEST2_C_150</t>
+  </si>
+  <si>
+    <t>BEST2_C_151</t>
+  </si>
+  <si>
+    <t>BEST2_C_152</t>
+  </si>
+  <si>
+    <t>BEST2_C_153</t>
+  </si>
+  <si>
+    <t>BEST2_C_154</t>
+  </si>
+  <si>
+    <t>BEST2_C_155</t>
+  </si>
+  <si>
+    <t>BEST2_C_156</t>
+  </si>
+  <si>
+    <t>BEST2_C_157</t>
+  </si>
+  <si>
+    <t>BEST2_C_158</t>
+  </si>
+  <si>
+    <t>BEST2_C_159</t>
+  </si>
+  <si>
+    <t>BEST2_C_160</t>
+  </si>
+  <si>
+    <t>BEST2_C_161</t>
+  </si>
+  <si>
+    <t>BEST2_C_162</t>
+  </si>
+  <si>
+    <t>BEST2_C_163</t>
+  </si>
+  <si>
+    <t>BEST2_C_164</t>
+  </si>
+  <si>
+    <t>BEST2_C_165</t>
+  </si>
+  <si>
+    <t>BEST2_C_166</t>
+  </si>
+  <si>
+    <t>BEST2_C_167</t>
+  </si>
+  <si>
+    <t>BEST2_C_168</t>
+  </si>
+  <si>
+    <t>BEST2_C_169</t>
+  </si>
+  <si>
+    <t>BEST2_C_170</t>
+  </si>
+  <si>
+    <t>BEST2_C_171</t>
+  </si>
+  <si>
+    <t>BEST2_C_172</t>
+  </si>
+  <si>
+    <t>BEST2_C_173</t>
+  </si>
+  <si>
+    <t>BEST2_C_174</t>
+  </si>
+  <si>
+    <t>BEST2_C_175</t>
+  </si>
+  <si>
+    <t>BEST2_C_176</t>
+  </si>
+  <si>
+    <t>BEST2_C_177</t>
+  </si>
+  <si>
+    <t>BEST2_C_178</t>
+  </si>
+  <si>
+    <t>BEST2_C_179</t>
+  </si>
+  <si>
+    <t>BEST2_C_180</t>
+  </si>
+  <si>
+    <t>BEST2_C_181</t>
+  </si>
+  <si>
+    <t>BEST2_C_182</t>
+  </si>
+  <si>
+    <t>BEST2_C_183</t>
+  </si>
+  <si>
+    <t>BEST2_C_184</t>
+  </si>
+  <si>
+    <t>BEST2_C_185</t>
+  </si>
+  <si>
+    <t>BEST2_C_186</t>
+  </si>
+  <si>
+    <t>BEST2_C_187</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,6 +647,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -993,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1004,13 +1011,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>202</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1054,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1107,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>354</v>
@@ -1160,7 +1167,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1833</v>
@@ -1213,7 +1220,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>839</v>
@@ -1266,7 +1273,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1319,7 +1326,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>106</v>
@@ -1372,7 +1379,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>146</v>
@@ -1425,7 +1432,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>2674</v>
@@ -1478,7 +1485,7 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>797</v>
@@ -1531,7 +1538,7 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>882</v>
@@ -1584,7 +1591,7 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1637,7 +1644,7 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>436</v>
@@ -1690,7 +1697,7 @@
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>1563</v>
@@ -1743,7 +1750,7 @@
         <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>195</v>
@@ -1796,7 +1803,7 @@
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>351</v>
@@ -1849,7 +1856,7 @@
         <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>444</v>
@@ -1902,7 +1909,7 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>41</v>
@@ -1955,7 +1962,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <v>365</v>
@@ -2008,7 +2015,7 @@
         <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>18</v>
@@ -2061,7 +2068,7 @@
         <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>306</v>
@@ -2114,7 +2121,7 @@
         <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C22">
         <v>1023</v>
@@ -2167,7 +2174,7 @@
         <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2220,7 +2227,7 @@
         <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C24">
         <v>2909</v>
@@ -2273,7 +2280,7 @@
         <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C25">
         <v>61</v>
@@ -2326,7 +2333,7 @@
         <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>1814</v>
@@ -2379,7 +2386,7 @@
         <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2432,7 +2439,7 @@
         <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2485,7 +2492,7 @@
         <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -2538,7 +2545,7 @@
         <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C30">
         <v>1458</v>
@@ -2591,7 +2598,7 @@
         <v>130</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -2644,7 +2651,7 @@
         <v>131</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C32">
         <v>347</v>
@@ -2697,7 +2704,7 @@
         <v>132</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C33">
         <v>335</v>
@@ -2750,7 +2757,7 @@
         <v>133</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C34">
         <v>550</v>
@@ -2803,7 +2810,7 @@
         <v>134</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C35">
         <v>11</v>
@@ -2856,7 +2863,7 @@
         <v>139</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C36">
         <v>72</v>
@@ -2909,7 +2916,7 @@
         <v>142</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C37">
         <v>48</v>
@@ -2962,7 +2969,7 @@
         <v>146</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C38">
         <v>549</v>
@@ -3015,7 +3022,7 @@
         <v>148</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -3068,7 +3075,7 @@
         <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -3121,7 +3128,7 @@
         <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -3174,7 +3181,7 @@
         <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C42">
         <v>53</v>
@@ -3227,7 +3234,7 @@
         <v>164</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C43">
         <v>2841</v>
@@ -3280,7 +3287,7 @@
         <v>166</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C44">
         <v>50</v>
@@ -3333,7 +3340,7 @@
         <v>168</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C45">
         <v>610</v>
@@ -3386,7 +3393,7 @@
         <v>171</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C46">
         <v>1792</v>
@@ -3439,7 +3446,7 @@
         <v>172</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C47">
         <v>2189</v>
@@ -3492,7 +3499,7 @@
         <v>179</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C48">
         <v>182</v>
@@ -3545,7 +3552,7 @@
         <v>181</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C49">
         <v>1506</v>
@@ -3598,7 +3605,7 @@
         <v>183</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -3651,7 +3658,7 @@
         <v>190</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C51">
         <v>538</v>
@@ -3704,7 +3711,7 @@
         <v>193</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C52">
         <v>5</v>
@@ -3757,7 +3764,7 @@
         <v>194</v>
       </c>
       <c r="B53" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C53">
         <v>550</v>
@@ -3810,7 +3817,7 @@
         <v>197</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C54">
         <v>696</v>
@@ -3863,7 +3870,7 @@
         <v>210</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3916,7 +3923,7 @@
         <v>212</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C56">
         <v>1197</v>
@@ -3969,7 +3976,7 @@
         <v>215</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -4022,7 +4029,7 @@
         <v>220</v>
       </c>
       <c r="B58" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C58">
         <v>30</v>
@@ -4075,7 +4082,7 @@
         <v>225</v>
       </c>
       <c r="B59" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C59">
         <v>4</v>
@@ -4128,7 +4135,7 @@
         <v>232</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -4181,7 +4188,7 @@
         <v>236</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -4234,7 +4241,7 @@
         <v>238</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C62">
         <v>42</v>
@@ -4287,7 +4294,7 @@
         <v>247</v>
       </c>
       <c r="B63" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -4340,7 +4347,7 @@
         <v>249</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C64">
         <v>42</v>
@@ -4393,7 +4400,7 @@
         <v>250</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C65">
         <v>558</v>
@@ -4446,7 +4453,7 @@
         <v>257</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C66">
         <v>285</v>
@@ -4499,7 +4506,7 @@
         <v>263</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C67">
         <v>72</v>
@@ -4552,7 +4559,7 @@
         <v>264</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C68">
         <v>127</v>
@@ -4605,7 +4612,7 @@
         <v>266</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C69">
         <v>359</v>
@@ -4658,7 +4665,7 @@
         <v>267</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C70">
         <v>630</v>
@@ -4711,7 +4718,7 @@
         <v>272</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C71">
         <v>1603</v>
@@ -4764,7 +4771,7 @@
         <v>273</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C72">
         <v>58</v>
@@ -4817,7 +4824,7 @@
         <v>276</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C73">
         <v>705</v>
@@ -4870,7 +4877,7 @@
         <v>277</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C74">
         <v>640</v>
@@ -4923,7 +4930,7 @@
         <v>279</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C75">
         <v>724</v>
@@ -4976,7 +4983,7 @@
         <v>280</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C76">
         <v>1891</v>
@@ -5029,7 +5036,7 @@
         <v>281</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C77">
         <v>1778</v>
@@ -5082,7 +5089,7 @@
         <v>284</v>
       </c>
       <c r="B78" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C78">
         <v>2463</v>
@@ -5135,7 +5142,7 @@
         <v>285</v>
       </c>
       <c r="B79" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C79">
         <v>693</v>
@@ -5188,7 +5195,7 @@
         <v>286</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C80">
         <v>1087</v>
@@ -5241,7 +5248,7 @@
         <v>289</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C81">
         <v>424</v>
@@ -5294,7 +5301,7 @@
         <v>293</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -5347,7 +5354,7 @@
         <v>295</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C83">
         <v>399</v>
@@ -5400,7 +5407,7 @@
         <v>299</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C84">
         <v>521</v>
@@ -5453,7 +5460,7 @@
         <v>301</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C85">
         <v>273</v>
@@ -5506,7 +5513,7 @@
         <v>304</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -5559,7 +5566,7 @@
         <v>311</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C87">
         <v>113</v>
@@ -5612,7 +5619,7 @@
         <v>312</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C88">
         <v>415</v>
@@ -5665,7 +5672,7 @@
         <v>314</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C89">
         <v>4752</v>
@@ -5718,7 +5725,7 @@
         <v>315</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C90">
         <v>291</v>
@@ -5771,7 +5778,7 @@
         <v>316</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C91">
         <v>155</v>
@@ -5824,7 +5831,7 @@
         <v>319</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C92">
         <v>489</v>
@@ -5877,7 +5884,7 @@
         <v>322</v>
       </c>
       <c r="B93" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C93">
         <v>1745</v>
@@ -5930,7 +5937,7 @@
         <v>325</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -5983,7 +5990,7 @@
         <v>327</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C95">
         <v>2065</v>
@@ -6036,7 +6043,7 @@
         <v>328</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C96">
         <v>89</v>
@@ -6089,7 +6096,7 @@
         <v>333</v>
       </c>
       <c r="B97" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C97">
         <v>2054</v>
@@ -6142,7 +6149,7 @@
         <v>334</v>
       </c>
       <c r="B98" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C98">
         <v>628</v>
@@ -6195,7 +6202,7 @@
         <v>335</v>
       </c>
       <c r="B99" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C99">
         <v>61</v>
@@ -6248,7 +6255,7 @@
         <v>336</v>
       </c>
       <c r="B100" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C100">
         <v>130</v>
@@ -6301,7 +6308,7 @@
         <v>338</v>
       </c>
       <c r="B101" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C101">
         <v>1349</v>
@@ -6354,7 +6361,7 @@
         <v>340</v>
       </c>
       <c r="B102" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C102">
         <v>58</v>
@@ -6407,7 +6414,7 @@
         <v>349</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C103">
         <v>982</v>
@@ -6460,7 +6467,7 @@
         <v>351</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C104">
         <v>2035</v>
@@ -6513,7 +6520,7 @@
         <v>353</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -6566,7 +6573,7 @@
         <v>355</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -6619,7 +6626,7 @@
         <v>358</v>
       </c>
       <c r="B107" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C107">
         <v>53</v>
@@ -6672,7 +6679,7 @@
         <v>360</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C108">
         <v>16</v>
@@ -6725,7 +6732,7 @@
         <v>362</v>
       </c>
       <c r="B109" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C109">
         <v>1082</v>
@@ -6778,7 +6785,7 @@
         <v>367</v>
       </c>
       <c r="B110" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C110">
         <v>131</v>
@@ -6831,7 +6838,7 @@
         <v>371</v>
       </c>
       <c r="B111" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C111">
         <v>837</v>
@@ -6884,7 +6891,7 @@
         <v>372</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C112">
         <v>89</v>
@@ -6937,7 +6944,7 @@
         <v>373</v>
       </c>
       <c r="B113" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C113">
         <v>62</v>
@@ -6990,7 +6997,7 @@
         <v>374</v>
       </c>
       <c r="B114" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C114">
         <v>6</v>
@@ -7043,7 +7050,7 @@
         <v>383</v>
       </c>
       <c r="B115" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C115">
         <v>186</v>
@@ -7096,7 +7103,7 @@
         <v>399</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C116">
         <v>1093</v>
@@ -7149,7 +7156,7 @@
         <v>407</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C117">
         <v>2808</v>
@@ -7202,7 +7209,7 @@
         <v>409</v>
       </c>
       <c r="B118" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C118">
         <v>2690</v>
@@ -7255,7 +7262,7 @@
         <v>411</v>
       </c>
       <c r="B119" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C119">
         <v>1539</v>
@@ -7308,7 +7315,7 @@
         <v>414</v>
       </c>
       <c r="B120" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C120">
         <v>283</v>
@@ -7361,7 +7368,7 @@
         <v>416</v>
       </c>
       <c r="B121" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C121">
         <v>1149</v>
@@ -7414,7 +7421,7 @@
         <v>420</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C122">
         <v>843</v>
@@ -7467,7 +7474,7 @@
         <v>425</v>
       </c>
       <c r="B123" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -7520,7 +7527,7 @@
         <v>426</v>
       </c>
       <c r="B124" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C124">
         <v>170</v>
@@ -7573,7 +7580,7 @@
         <v>427</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C125">
         <v>1563</v>
@@ -7626,7 +7633,7 @@
         <v>429</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C126">
         <v>360</v>
@@ -7679,7 +7686,7 @@
         <v>436</v>
       </c>
       <c r="B127" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C127">
         <v>948</v>
@@ -7732,7 +7739,7 @@
         <v>438</v>
       </c>
       <c r="B128" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C128">
         <v>46</v>
@@ -7785,7 +7792,7 @@
         <v>443</v>
       </c>
       <c r="B129" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C129">
         <v>453</v>
@@ -7838,7 +7845,7 @@
         <v>447</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C130">
         <v>216</v>
@@ -7891,7 +7898,7 @@
         <v>449</v>
       </c>
       <c r="B131" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C131">
         <v>335</v>
@@ -7944,7 +7951,7 @@
         <v>453</v>
       </c>
       <c r="B132" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C132">
         <v>2490</v>
@@ -7997,7 +8004,7 @@
         <v>457</v>
       </c>
       <c r="B133" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -8050,7 +8057,7 @@
         <v>460</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -8103,7 +8110,7 @@
         <v>463</v>
       </c>
       <c r="B135" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C135">
         <v>1140</v>
@@ -8156,7 +8163,7 @@
         <v>464</v>
       </c>
       <c r="B136" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C136">
         <v>1038</v>
@@ -8209,7 +8216,7 @@
         <v>472</v>
       </c>
       <c r="B137" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -8262,7 +8269,7 @@
         <v>476</v>
       </c>
       <c r="B138" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C138">
         <v>3</v>
@@ -8315,7 +8322,7 @@
         <v>477</v>
       </c>
       <c r="B139" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C139">
         <v>1681</v>
@@ -8368,7 +8375,7 @@
         <v>480</v>
       </c>
       <c r="B140" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C140">
         <v>204</v>
@@ -8421,7 +8428,7 @@
         <v>483</v>
       </c>
       <c r="B141" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C141">
         <v>140</v>
@@ -8474,7 +8481,7 @@
         <v>487</v>
       </c>
       <c r="B142" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C142">
         <v>2891</v>
@@ -8527,7 +8534,7 @@
         <v>493</v>
       </c>
       <c r="B143" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C143">
         <v>411</v>
@@ -8580,7 +8587,7 @@
         <v>499</v>
       </c>
       <c r="B144" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C144">
         <v>167</v>
@@ -8633,7 +8640,7 @@
         <v>502</v>
       </c>
       <c r="B145" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C145">
         <v>251</v>
@@ -8686,7 +8693,7 @@
         <v>503</v>
       </c>
       <c r="B146" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C146">
         <v>2177</v>
@@ -8739,7 +8746,7 @@
         <v>505</v>
       </c>
       <c r="B147" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C147">
         <v>362</v>
@@ -8792,7 +8799,7 @@
         <v>511</v>
       </c>
       <c r="B148" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C148">
         <v>1372</v>
@@ -8845,7 +8852,7 @@
         <v>517</v>
       </c>
       <c r="B149" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -8898,7 +8905,7 @@
         <v>519</v>
       </c>
       <c r="B150" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C150">
         <v>409</v>
@@ -8951,7 +8958,7 @@
         <v>528</v>
       </c>
       <c r="B151" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C151">
         <v>1044</v>
@@ -9004,7 +9011,7 @@
         <v>538</v>
       </c>
       <c r="B152" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C152">
         <v>71</v>
@@ -9057,7 +9064,7 @@
         <v>540</v>
       </c>
       <c r="B153" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C153">
         <v>655</v>
@@ -9110,7 +9117,7 @@
         <v>552</v>
       </c>
       <c r="B154" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C154">
         <v>5</v>
@@ -9163,7 +9170,7 @@
         <v>566</v>
       </c>
       <c r="B155" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C155">
         <v>1441</v>
@@ -9216,7 +9223,7 @@
         <v>567</v>
       </c>
       <c r="B156" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C156">
         <v>5</v>
@@ -9269,7 +9276,7 @@
         <v>568</v>
       </c>
       <c r="B157" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C157">
         <v>67</v>
@@ -9322,7 +9329,7 @@
         <v>580</v>
       </c>
       <c r="B158" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C158">
         <v>97</v>
@@ -9375,7 +9382,7 @@
         <v>588</v>
       </c>
       <c r="B159" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C159">
         <v>919</v>
@@ -9428,7 +9435,7 @@
         <v>591</v>
       </c>
       <c r="B160" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C160">
         <v>2</v>
@@ -9481,7 +9488,7 @@
         <v>592</v>
       </c>
       <c r="B161" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C161">
         <v>7</v>
@@ -9534,7 +9541,7 @@
         <v>593</v>
       </c>
       <c r="B162" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C162">
         <v>1074</v>
@@ -9587,7 +9594,7 @@
         <v>595</v>
       </c>
       <c r="B163" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C163">
         <v>673</v>
@@ -9640,7 +9647,7 @@
         <v>600</v>
       </c>
       <c r="B164" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C164">
         <v>55</v>
@@ -9693,7 +9700,7 @@
         <v>604</v>
       </c>
       <c r="B165" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C165">
         <v>1127</v>
@@ -9746,7 +9753,7 @@
         <v>605</v>
       </c>
       <c r="B166" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C166">
         <v>1046</v>
@@ -9799,7 +9806,7 @@
         <v>608</v>
       </c>
       <c r="B167" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C167">
         <v>129</v>
@@ -9852,7 +9859,7 @@
         <v>609</v>
       </c>
       <c r="B168" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C168">
         <v>542</v>
@@ -9905,7 +9912,7 @@
         <v>616</v>
       </c>
       <c r="B169" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C169">
         <v>186</v>
@@ -9958,7 +9965,7 @@
         <v>619</v>
       </c>
       <c r="B170" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C170">
         <v>206</v>
@@ -10011,7 +10018,7 @@
         <v>622</v>
       </c>
       <c r="B171" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C171">
         <v>950</v>
@@ -10064,7 +10071,7 @@
         <v>629</v>
       </c>
       <c r="B172" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C172">
         <v>0</v>
@@ -10117,7 +10124,7 @@
         <v>637</v>
       </c>
       <c r="B173" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -10170,7 +10177,7 @@
         <v>641</v>
       </c>
       <c r="B174" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C174">
         <v>2840</v>
@@ -10223,7 +10230,7 @@
         <v>643</v>
       </c>
       <c r="B175" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C175">
         <v>1692</v>
@@ -10276,7 +10283,7 @@
         <v>646</v>
       </c>
       <c r="B176" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C176">
         <v>6</v>
@@ -10329,7 +10336,7 @@
         <v>647</v>
       </c>
       <c r="B177" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C177">
         <v>121</v>
@@ -10382,7 +10389,7 @@
         <v>648</v>
       </c>
       <c r="B178" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C178">
         <v>248</v>
@@ -10435,7 +10442,7 @@
         <v>651</v>
       </c>
       <c r="B179" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C179">
         <v>825</v>
@@ -10488,7 +10495,7 @@
         <v>652</v>
       </c>
       <c r="B180" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C180">
         <v>2471</v>
@@ -10541,7 +10548,7 @@
         <v>655</v>
       </c>
       <c r="B181" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C181">
         <v>1609</v>
@@ -10594,7 +10601,7 @@
         <v>666</v>
       </c>
       <c r="B182" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C182">
         <v>1425</v>
@@ -10647,7 +10654,7 @@
         <v>667</v>
       </c>
       <c r="B183" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C183">
         <v>75</v>
@@ -10700,7 +10707,7 @@
         <v>668</v>
       </c>
       <c r="B184" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C184">
         <v>1033</v>
@@ -10753,7 +10760,7 @@
         <v>682</v>
       </c>
       <c r="B185" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C185">
         <v>0</v>
@@ -10806,7 +10813,7 @@
         <v>685</v>
       </c>
       <c r="B186" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C186">
         <v>254</v>
@@ -10859,7 +10866,7 @@
         <v>686</v>
       </c>
       <c r="B187" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C187">
         <v>1621</v>
@@ -10912,7 +10919,7 @@
         <v>689</v>
       </c>
       <c r="B188" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -10961,6 +10968,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>